<commit_message>
Add base Frame work
small  test
</commit_message>
<xml_diff>
--- a/GameAwards2020/Assets/GameMain/DataTables/Excel/Scene.xlsx
+++ b/GameAwards2020/Assets/GameMain/DataTables/Excel/Scene.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GameAwards2020\GameAwards2020\Assets\GameMain\DataTables\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8705DEF3-80E0-42D5-BF0F-41D68FEB0407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D52E52E-5C72-4FAE-92AB-6DCC38713D44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -58,6 +58,14 @@
   </si>
   <si>
     <t>BGM ID</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Menu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MainGame</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -126,18 +134,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -456,21 +467,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -478,34 +493,61 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>